<commit_message>
organised all modules into folders
</commit_message>
<xml_diff>
--- a/data/cash_flow.xlsx
+++ b/data/cash_flow.xlsx
@@ -736,10 +736,10 @@
         </is>
       </c>
       <c r="B26" s="0" t="n">
-        <v>-0.1623</v>
+        <v>-0.1621</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>-0.0958</v>
+        <v>-0.0959</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>-0.0401</v>

</xml_diff>